<commit_message>
BR cartacei e files
</commit_message>
<xml_diff>
--- a/Roma_BR/BR03/BR03_studenti.xlsx
+++ b/Roma_BR/BR03/BR03_studenti.xlsx
@@ -1,24 +1,465 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocpa\OneDrive\Documenti\GitHub\tragedynatural\Roma_BR\BR03\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F740A1-EAC0-4FBD-A201-465F10D4B71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="143">
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>IPAddress</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Duration (in seconds)</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>RecordedDate</t>
+  </si>
+  <si>
+    <t>ResponseId</t>
+  </si>
+  <si>
+    <t>RecipientLastName</t>
+  </si>
+  <si>
+    <t>RecipientFirstName</t>
+  </si>
+  <si>
+    <t>RecipientEmail</t>
+  </si>
+  <si>
+    <t>ExternalReference</t>
+  </si>
+  <si>
+    <t>LocationLatitude</t>
+  </si>
+  <si>
+    <t>LocationLongitude</t>
+  </si>
+  <si>
+    <t>DistributionChannel</t>
+  </si>
+  <si>
+    <t>UserLanguage</t>
+  </si>
+  <si>
+    <t>consenso_4</t>
+  </si>
+  <si>
+    <t>consenso_5</t>
+  </si>
+  <si>
+    <t>colore</t>
+  </si>
+  <si>
+    <t>sim_facile</t>
+  </si>
+  <si>
+    <t>sim_interessante</t>
+  </si>
+  <si>
+    <t>sim_imparato</t>
+  </si>
+  <si>
+    <t>sim_imparato2</t>
+  </si>
+  <si>
+    <t>collab_gruppo_1</t>
+  </si>
+  <si>
+    <t>collab_gruppo_2</t>
+  </si>
+  <si>
+    <t>collab_gruppo_3</t>
+  </si>
+  <si>
+    <t>sostenibilita</t>
+  </si>
+  <si>
+    <t>comp_sost_1</t>
+  </si>
+  <si>
+    <t>comp_sost_2</t>
+  </si>
+  <si>
+    <t>comp_sost_3</t>
+  </si>
+  <si>
+    <t>comp_sost_4</t>
+  </si>
+  <si>
+    <t>comp_sost_5</t>
+  </si>
+  <si>
+    <t>comp_sost_6</t>
+  </si>
+  <si>
+    <t>comp_sost2_1</t>
+  </si>
+  <si>
+    <t>comp_sost2_2</t>
+  </si>
+  <si>
+    <t>comp_sost2_3</t>
+  </si>
+  <si>
+    <t>collab_classe1_1</t>
+  </si>
+  <si>
+    <t>collab_classe1_2</t>
+  </si>
+  <si>
+    <t>collab_classe1_3</t>
+  </si>
+  <si>
+    <t>collab_classe1_4</t>
+  </si>
+  <si>
+    <t>collab_classe1_5</t>
+  </si>
+  <si>
+    <t>collab_classe2_1</t>
+  </si>
+  <si>
+    <t>collab_classe2_2</t>
+  </si>
+  <si>
+    <t>collab_classe2_3</t>
+  </si>
+  <si>
+    <t>collab_classe2_4</t>
+  </si>
+  <si>
+    <t>collab_classe2_5</t>
+  </si>
+  <si>
+    <t>collab_classe2_6</t>
+  </si>
+  <si>
+    <t>turn</t>
+  </si>
+  <si>
+    <t>smartphone</t>
+  </si>
+  <si>
+    <t>colore_stringa</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:35:36</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:38:47</t>
+  </si>
+  <si>
+    <t>78.209.31.214</t>
+  </si>
+  <si>
+    <t>R_2lcmcV8U95hbwCr</t>
+  </si>
+  <si>
+    <t>anonymous</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>che si deve lavare tutti insieme, bisogna collaborare</t>
+  </si>
+  <si>
+    <t>ridurre il più possibile il danneggiamento dell’ambiente</t>
+  </si>
+  <si>
+    <t>BR03</t>
+  </si>
+  <si>
+    <t>rosa</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:37:03</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:39:08</t>
+  </si>
+  <si>
+    <t>151.37.219.100</t>
+  </si>
+  <si>
+    <t>R_2jZpkMdTFcxElEY</t>
+  </si>
+  <si>
+    <t>azzurro</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:35:39</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:39:14</t>
+  </si>
+  <si>
+    <t>151.37.203.44</t>
+  </si>
+  <si>
+    <t>R_80DOZIywQejLIAN</t>
+  </si>
+  <si>
+    <t>Che bisogna trovare un equilibrio su risorse naturali e consumi</t>
+  </si>
+  <si>
+    <t>giallo</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:35:43</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:39:25</t>
+  </si>
+  <si>
+    <t>185.8.121.247</t>
+  </si>
+  <si>
+    <t>R_2wBqrZGkrZTNIR3</t>
+  </si>
+  <si>
+    <t>Astuzia,intelligenza e furbizia</t>
+  </si>
+  <si>
+    <t>Mantenere e riprovare</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:36:21</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:39:39</t>
+  </si>
+  <si>
+    <t>217.201.52.194</t>
+  </si>
+  <si>
+    <t>R_2isL5gTHixqUCkF</t>
+  </si>
+  <si>
+    <t>Che si deve fare attenzione su cosa spendi</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:37:23</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:40:23</t>
+  </si>
+  <si>
+    <t>151.35.146.74</t>
+  </si>
+  <si>
+    <t>R_8gS5FzKvvwCDGXT</t>
+  </si>
+  <si>
+    <t>Come gestire un pascolo</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:40:40</t>
+  </si>
+  <si>
+    <t>5.91.142.40</t>
+  </si>
+  <si>
+    <t>R_8rlwDvpL1AgmCD1</t>
+  </si>
+  <si>
+    <t>che bisogna collaborare tutti insieme</t>
+  </si>
+  <si>
+    <t>di ridurre il danneggiamento dell’ambiente</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:35:42</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:40:46</t>
+  </si>
+  <si>
+    <t>151.57.250.88</t>
+  </si>
+  <si>
+    <t>R_8S6qcK4iBfW9aBU</t>
+  </si>
+  <si>
+    <t>Che bisogna collaborare</t>
+  </si>
+  <si>
+    <t>La sostenibilità è ridurre il più possibile il danneggiamento dell’ambiente</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:38:16</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:40:48</t>
+  </si>
+  <si>
+    <t>151.43.218.225</t>
+  </si>
+  <si>
+    <t>R_2q3HHdPTaUXU0nN</t>
+  </si>
+  <si>
+    <t>blu</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:35:49</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:41:15</t>
+  </si>
+  <si>
+    <t>151.37.108.193</t>
+  </si>
+  <si>
+    <t>R_87Kh3zd3krA9Urf</t>
+  </si>
+  <si>
+    <t>La collaborazione</t>
+  </si>
+  <si>
+    <t>Ridurre il più possibile danneggiamento dell’ambiente</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:36:27</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:41:26</t>
+  </si>
+  <si>
+    <t>78.208.179.70</t>
+  </si>
+  <si>
+    <t>R_8VIiB5AVeK47yA9</t>
+  </si>
+  <si>
+    <t>Che è necessario collaborare per creare un ambiente sostenibile</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:35:51</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:42:37</t>
+  </si>
+  <si>
+    <t>5.91.140.149</t>
+  </si>
+  <si>
+    <t>R_8h0IyARECsrw2JS</t>
+  </si>
+  <si>
+    <t>Si ho capitol che biography colaborare di pic con I compagni</t>
+  </si>
+  <si>
+    <t>rosso</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:36:17</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:42:59</t>
+  </si>
+  <si>
+    <t>5.91.244.238</t>
+  </si>
+  <si>
+    <t>R_2f9aMikPuRfK7O7</t>
+  </si>
+  <si>
+    <t>Ho imparato che bisogna mettere più contributo comune per permettere di ottenere più pascolo per le mucche</t>
+  </si>
+  <si>
+    <t>sostenere qualcosa come una persona o un lavoro</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:43:02</t>
+  </si>
+  <si>
+    <t>R_8911eoEvaZXKOBP</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:43:07</t>
+  </si>
+  <si>
+    <t>37.163.54.206</t>
+  </si>
+  <si>
+    <t>R_27GVr9grygv7n21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ho imparato che bisogna mettere più contributo comune per permettere di ottenere più pascolo. _x000D_
+</t>
+  </si>
+  <si>
+    <t>Sostenere, una persona, un lavoro o un progetto</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:40:08</t>
+  </si>
+  <si>
+    <t>2024-11-27 11:43:13</t>
+  </si>
+  <si>
+    <t>78.211.195.11</t>
+  </si>
+  <si>
+    <t>R_8d9Mo3ypBC1zTUJ</t>
+  </si>
+  <si>
+    <t>Che si deve collaborare di più con i compagni</t>
+  </si>
+  <si>
+    <t>R_cartaceo_11</t>
+  </si>
+  <si>
+    <t>si deve collaborare di più con i compagni</t>
+  </si>
+  <si>
+    <t>sostiene qualunchue persona e aiutare sempre il prosimo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,13 +508,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -111,7 +560,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -145,6 +594,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -179,9 +629,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -354,291 +805,187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AY18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="24.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>StartDate</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>EndDate</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>IPAddress</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Progress</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Duration (in seconds)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Finished</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>RecordedDate</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>ResponseId</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>RecipientLastName</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>RecipientFirstName</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>RecipientEmail</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>ExternalReference</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>LocationLatitude</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>LocationLongitude</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>DistributionChannel</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>UserLanguage</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>consenso_4</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>consenso_5</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>colore</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>sim_facile</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>sim_interessante</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>sim_imparato</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>sim_imparato2</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>collab_gruppo_1</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>collab_gruppo_2</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>collab_gruppo_3</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>sostenibilita</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost_1</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost_2</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost_3</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost_4</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost_5</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost_6</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost2_1</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost2_2</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>comp_sost2_3</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe1_1</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe1_2</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe1_3</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe1_4</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe1_5</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe2_1</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe2_2</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe2_3</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe2_4</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe2_5</t>
-        </is>
-      </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>collab_classe2_6</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>turn</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>smartphone</t>
-        </is>
-      </c>
-      <c r="AY1" s="1" t="inlineStr">
-        <is>
-          <t>colore_stringa</t>
-        </is>
+    <row r="1" spans="1:51" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:35:36</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:38:47</t>
-        </is>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>78.209.31.214</t>
-        </is>
+      <c r="D2" t="s">
+        <v>53</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -650,12 +997,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="2">
-        <v>45623.48527954861</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>R_2lcmcV8U95hbwCr</t>
-        </is>
+        <v>45623.485279548608</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
       </c>
       <c r="N2">
         <v>43.1479</v>
@@ -663,25 +1008,17 @@
       <c r="O2">
         <v>12.1097</v>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S2" t="s">
+        <v>57</v>
       </c>
       <c r="T2">
         <v>4</v>
@@ -695,10 +1032,8 @@
       <c r="W2">
         <v>1</v>
       </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>che si deve lavare tutti insieme, bisogna collaborare</t>
-        </is>
+      <c r="X2" t="s">
+        <v>58</v>
       </c>
       <c r="Y2">
         <v>5</v>
@@ -709,10 +1044,8 @@
       <c r="AA2">
         <v>5</v>
       </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>ridurre il più possibile il danneggiamento dell’ambiente</t>
-        </is>
+      <c r="AB2" t="s">
+        <v>59</v>
       </c>
       <c r="AC2">
         <v>4</v>
@@ -774,38 +1107,28 @@
       <c r="AV2">
         <v>1</v>
       </c>
-      <c r="AW2" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW2" t="s">
+        <v>60</v>
       </c>
       <c r="AX2">
         <v>1</v>
       </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>rosa</t>
-        </is>
+      <c r="AY2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:37:03</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:39:08</t>
-        </is>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>151.37.219.100</t>
-        </is>
+      <c r="D3" t="s">
+        <v>64</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -817,38 +1140,28 @@
         <v>1</v>
       </c>
       <c r="H3" s="2">
-        <v>45623.48552542824</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>R_2jZpkMdTFcxElEY</t>
-        </is>
+        <v>45623.485525428237</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
       </c>
       <c r="N3">
-        <v>41.9008</v>
+        <v>41.900799999999997</v>
       </c>
       <c r="O3">
-        <v>12.4874</v>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+        <v>12.487399999999999</v>
+      </c>
+      <c r="P3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" t="s">
+        <v>57</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -865,38 +1178,28 @@
       <c r="AL3">
         <v>1</v>
       </c>
-      <c r="AW3" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW3" t="s">
+        <v>60</v>
       </c>
       <c r="AX3">
         <v>1</v>
       </c>
-      <c r="AY3" t="inlineStr">
-        <is>
-          <t>azzurro</t>
-        </is>
+      <c r="AY3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:35:39</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:39:14</t>
-        </is>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>151.37.203.44</t>
-        </is>
+      <c r="D4" t="s">
+        <v>69</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -908,38 +1211,28 @@
         <v>1</v>
       </c>
       <c r="H4" s="2">
-        <v>45623.48559425926</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>R_80DOZIywQejLIAN</t>
-        </is>
+        <v>45623.485594259262</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
       </c>
       <c r="N4">
-        <v>41.9008</v>
+        <v>41.900799999999997</v>
       </c>
       <c r="O4">
-        <v>12.4874</v>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+        <v>12.487399999999999</v>
+      </c>
+      <c r="P4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>56</v>
+      </c>
+      <c r="R4" t="s">
+        <v>57</v>
+      </c>
+      <c r="S4" t="s">
+        <v>57</v>
       </c>
       <c r="T4">
         <v>3</v>
@@ -953,10 +1246,8 @@
       <c r="W4">
         <v>1</v>
       </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Che bisogna trovare un equilibrio su risorse naturali e consumi</t>
-        </is>
+      <c r="X4" t="s">
+        <v>71</v>
       </c>
       <c r="Y4">
         <v>5</v>
@@ -1027,38 +1318,28 @@
       <c r="AV4">
         <v>2</v>
       </c>
-      <c r="AW4" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW4" t="s">
+        <v>60</v>
       </c>
       <c r="AX4">
         <v>1</v>
       </c>
-      <c r="AY4" t="inlineStr">
-        <is>
-          <t>giallo</t>
-        </is>
+      <c r="AY4" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:35:43</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:39:25</t>
-        </is>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>185.8.121.247</t>
-        </is>
+      <c r="D5" t="s">
+        <v>75</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -1070,12 +1351,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="2">
-        <v>45623.48571982639</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>R_2wBqrZGkrZTNIR3</t>
-        </is>
+        <v>45623.485719826393</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
       </c>
       <c r="N5">
         <v>43.1479</v>
@@ -1083,25 +1362,17 @@
       <c r="O5">
         <v>12.1097</v>
       </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" t="s">
+        <v>57</v>
+      </c>
+      <c r="S5" t="s">
+        <v>57</v>
       </c>
       <c r="T5">
         <v>3</v>
@@ -1115,10 +1386,8 @@
       <c r="W5">
         <v>1</v>
       </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>Astuzia,intelligenza e furbizia</t>
-        </is>
+      <c r="X5" t="s">
+        <v>77</v>
       </c>
       <c r="Y5">
         <v>5</v>
@@ -1129,10 +1398,8 @@
       <c r="AA5">
         <v>1</v>
       </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>Mantenere e riprovare</t>
-        </is>
+      <c r="AB5" t="s">
+        <v>78</v>
       </c>
       <c r="AC5">
         <v>5</v>
@@ -1194,38 +1461,28 @@
       <c r="AV5">
         <v>7</v>
       </c>
-      <c r="AW5" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW5" t="s">
+        <v>60</v>
       </c>
       <c r="AX5">
         <v>1</v>
       </c>
-      <c r="AY5" t="inlineStr">
-        <is>
-          <t>giallo</t>
-        </is>
+      <c r="AY5" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:36:21</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:39:39</t>
-        </is>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>217.201.52.194</t>
-        </is>
+      <c r="D6" t="s">
+        <v>81</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -1237,38 +1494,28 @@
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>45623.48588224537</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>R_2isL5gTHixqUCkF</t>
-        </is>
+        <v>45623.485882245368</v>
+      </c>
+      <c r="I6" t="s">
+        <v>82</v>
       </c>
       <c r="N6">
         <v>41.8904</v>
       </c>
       <c r="O6">
-        <v>12.5126</v>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+        <v>12.512600000000001</v>
+      </c>
+      <c r="P6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6" t="s">
+        <v>57</v>
       </c>
       <c r="T6">
         <v>3</v>
@@ -1282,10 +1529,8 @@
       <c r="W6">
         <v>1</v>
       </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>Che si deve fare attenzione su cosa spendi</t>
-        </is>
+      <c r="X6" t="s">
+        <v>83</v>
       </c>
       <c r="Y6">
         <v>5</v>
@@ -1356,38 +1601,28 @@
       <c r="AV6">
         <v>6</v>
       </c>
-      <c r="AW6" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW6" t="s">
+        <v>60</v>
       </c>
       <c r="AX6">
         <v>1</v>
       </c>
-      <c r="AY6" t="inlineStr">
-        <is>
-          <t>giallo</t>
-        </is>
+      <c r="AY6" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:37:23</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:40:23</t>
-        </is>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>151.35.146.74</t>
-        </is>
+      <c r="D7" t="s">
+        <v>86</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -1399,12 +1634,10 @@
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <v>45623.48638364583</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>R_8gS5FzKvvwCDGXT</t>
-        </is>
+        <v>45623.486383645832</v>
+      </c>
+      <c r="I7" t="s">
+        <v>87</v>
       </c>
       <c r="N7">
         <v>43.1479</v>
@@ -1412,25 +1645,17 @@
       <c r="O7">
         <v>12.1097</v>
       </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R7" t="s">
+        <v>57</v>
+      </c>
+      <c r="S7" t="s">
+        <v>57</v>
       </c>
       <c r="T7">
         <v>1</v>
@@ -1444,10 +1669,8 @@
       <c r="W7">
         <v>1</v>
       </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>Come gestire un pascolo</t>
-        </is>
+      <c r="X7" t="s">
+        <v>88</v>
       </c>
       <c r="Y7">
         <v>5</v>
@@ -1512,38 +1735,28 @@
       <c r="AV7">
         <v>1</v>
       </c>
-      <c r="AW7" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW7" t="s">
+        <v>60</v>
       </c>
       <c r="AX7">
         <v>1</v>
       </c>
-      <c r="AY7" t="inlineStr">
-        <is>
-          <t>azzurro</t>
-        </is>
+      <c r="AY7" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:35:43</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:40:40</t>
-        </is>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>5.91.142.40</t>
-        </is>
+      <c r="D8" t="s">
+        <v>90</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -1555,38 +1768,28 @@
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <v>45623.48658377315</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>R_8rlwDvpL1AgmCD1</t>
-        </is>
+        <v>45623.486583773149</v>
+      </c>
+      <c r="I8" t="s">
+        <v>91</v>
       </c>
       <c r="N8">
         <v>41.8904</v>
       </c>
       <c r="O8">
-        <v>12.5126</v>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+        <v>12.512600000000001</v>
+      </c>
+      <c r="P8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" t="s">
+        <v>57</v>
       </c>
       <c r="T8">
         <v>4</v>
@@ -1600,10 +1803,8 @@
       <c r="W8">
         <v>1</v>
       </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>che bisogna collaborare tutti insieme</t>
-        </is>
+      <c r="X8" t="s">
+        <v>92</v>
       </c>
       <c r="Y8">
         <v>5</v>
@@ -1614,10 +1815,8 @@
       <c r="AA8">
         <v>5</v>
       </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>di ridurre il danneggiamento dell’ambiente</t>
-        </is>
+      <c r="AB8" t="s">
+        <v>93</v>
       </c>
       <c r="AC8">
         <v>3</v>
@@ -1679,38 +1878,28 @@
       <c r="AV8">
         <v>6</v>
       </c>
-      <c r="AW8" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW8" t="s">
+        <v>60</v>
       </c>
       <c r="AX8">
         <v>1</v>
       </c>
-      <c r="AY8" t="inlineStr">
-        <is>
-          <t>rosa</t>
-        </is>
+      <c r="AY8" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:35:42</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:40:46</t>
-        </is>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>151.57.250.88</t>
-        </is>
+      <c r="D9" t="s">
+        <v>96</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -1722,12 +1911,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <v>45623.48665571759</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>R_8S6qcK4iBfW9aBU</t>
-        </is>
+        <v>45623.486655717592</v>
+      </c>
+      <c r="I9" t="s">
+        <v>97</v>
       </c>
       <c r="N9">
         <v>43.1479</v>
@@ -1735,25 +1922,17 @@
       <c r="O9">
         <v>12.1097</v>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>56</v>
+      </c>
+      <c r="R9" t="s">
+        <v>57</v>
+      </c>
+      <c r="S9" t="s">
+        <v>57</v>
       </c>
       <c r="T9">
         <v>4</v>
@@ -1767,10 +1946,8 @@
       <c r="W9">
         <v>1</v>
       </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>Che bisogna collaborare</t>
-        </is>
+      <c r="X9" t="s">
+        <v>98</v>
       </c>
       <c r="Y9">
         <v>5</v>
@@ -1781,10 +1958,8 @@
       <c r="AA9">
         <v>5</v>
       </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>La sostenibilità è ridurre il più possibile il danneggiamento dell’ambiente</t>
-        </is>
+      <c r="AB9" t="s">
+        <v>99</v>
       </c>
       <c r="AC9">
         <v>5</v>
@@ -1846,38 +2021,28 @@
       <c r="AV9">
         <v>8</v>
       </c>
-      <c r="AW9" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW9" t="s">
+        <v>60</v>
       </c>
       <c r="AX9">
         <v>1</v>
       </c>
-      <c r="AY9" t="inlineStr">
-        <is>
-          <t>rosa</t>
-        </is>
+      <c r="AY9" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:38:16</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:40:48</t>
-        </is>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>151.43.218.225</t>
-        </is>
+      <c r="D10" t="s">
+        <v>102</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -1889,12 +2054,10 @@
         <v>1</v>
       </c>
       <c r="H10" s="2">
-        <v>45623.48668289352</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>R_2q3HHdPTaUXU0nN</t>
-        </is>
+        <v>45623.486682893519</v>
+      </c>
+      <c r="I10" t="s">
+        <v>103</v>
       </c>
       <c r="N10">
         <v>43.1479</v>
@@ -1902,25 +2065,17 @@
       <c r="O10">
         <v>12.1097</v>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P10" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" t="s">
+        <v>57</v>
+      </c>
+      <c r="S10" t="s">
+        <v>57</v>
       </c>
       <c r="T10">
         <v>2</v>
@@ -1982,38 +2137,28 @@
       <c r="AT10">
         <v>8</v>
       </c>
-      <c r="AW10" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW10" t="s">
+        <v>60</v>
       </c>
       <c r="AX10">
         <v>1</v>
       </c>
-      <c r="AY10" t="inlineStr">
-        <is>
-          <t>blu</t>
-        </is>
+      <c r="AY10" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:35:49</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:41:15</t>
-        </is>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>151.37.108.193</t>
-        </is>
+      <c r="D11" t="s">
+        <v>107</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -2025,12 +2170,10 @@
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <v>45623.48699077546</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>R_87Kh3zd3krA9Urf</t>
-        </is>
+        <v>45623.486990775462</v>
+      </c>
+      <c r="I11" t="s">
+        <v>108</v>
       </c>
       <c r="N11">
         <v>43.1479</v>
@@ -2038,25 +2181,17 @@
       <c r="O11">
         <v>12.1097</v>
       </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P11" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>56</v>
+      </c>
+      <c r="R11" t="s">
+        <v>57</v>
+      </c>
+      <c r="S11" t="s">
+        <v>57</v>
       </c>
       <c r="T11">
         <v>4</v>
@@ -2070,10 +2205,8 @@
       <c r="W11">
         <v>1</v>
       </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>La collaborazione</t>
-        </is>
+      <c r="X11" t="s">
+        <v>109</v>
       </c>
       <c r="Y11">
         <v>5</v>
@@ -2084,10 +2217,8 @@
       <c r="AA11">
         <v>5</v>
       </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>Ridurre il più possibile danneggiamento dell’ambiente</t>
-        </is>
+      <c r="AB11" t="s">
+        <v>110</v>
       </c>
       <c r="AC11">
         <v>5</v>
@@ -2149,38 +2280,28 @@
       <c r="AV11">
         <v>6</v>
       </c>
-      <c r="AW11" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW11" t="s">
+        <v>60</v>
       </c>
       <c r="AX11">
         <v>1</v>
       </c>
-      <c r="AY11" t="inlineStr">
-        <is>
-          <t>rosa</t>
-        </is>
+      <c r="AY11" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:36:27</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:41:26</t>
-        </is>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>78.208.179.70</t>
-        </is>
+      <c r="D12" t="s">
+        <v>113</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -2192,38 +2313,28 @@
         <v>1</v>
       </c>
       <c r="H12" s="2">
-        <v>45623.48712024305</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>R_8VIiB5AVeK47yA9</t>
-        </is>
+        <v>45623.487120243051</v>
+      </c>
+      <c r="I12" t="s">
+        <v>114</v>
       </c>
       <c r="N12">
-        <v>45.4722</v>
+        <v>45.472200000000001</v>
       </c>
       <c r="O12">
-        <v>9.1922</v>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+        <v>9.1921999999999997</v>
+      </c>
+      <c r="P12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R12" t="s">
+        <v>57</v>
+      </c>
+      <c r="S12" t="s">
+        <v>57</v>
       </c>
       <c r="T12">
         <v>1</v>
@@ -2237,10 +2348,8 @@
       <c r="W12">
         <v>1</v>
       </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>Che è necessario collaborare per creare un ambiente sostenibile</t>
-        </is>
+      <c r="X12" t="s">
+        <v>115</v>
       </c>
       <c r="Y12">
         <v>4</v>
@@ -2311,38 +2420,28 @@
       <c r="AV12">
         <v>2</v>
       </c>
-      <c r="AW12" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW12" t="s">
+        <v>60</v>
       </c>
       <c r="AX12">
         <v>1</v>
       </c>
-      <c r="AY12" t="inlineStr">
-        <is>
-          <t>azzurro</t>
-        </is>
+      <c r="AY12" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:35:51</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:42:37</t>
-        </is>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>5.91.140.149</t>
-        </is>
+      <c r="D13" t="s">
+        <v>118</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -2354,38 +2453,28 @@
         <v>1</v>
       </c>
       <c r="H13" s="2">
-        <v>45623.48793615741</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>R_8h0IyARECsrw2JS</t>
-        </is>
+        <v>45623.487936157413</v>
+      </c>
+      <c r="I13" t="s">
+        <v>119</v>
       </c>
       <c r="N13">
         <v>41.8904</v>
       </c>
       <c r="O13">
-        <v>12.5126</v>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+        <v>12.512600000000001</v>
+      </c>
+      <c r="P13" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>56</v>
+      </c>
+      <c r="R13" t="s">
+        <v>57</v>
+      </c>
+      <c r="S13" t="s">
+        <v>57</v>
       </c>
       <c r="T13">
         <v>5</v>
@@ -2399,10 +2488,8 @@
       <c r="W13">
         <v>1</v>
       </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>Si ho capitol che biography colaborare di pic con I compagni</t>
-        </is>
+      <c r="X13" t="s">
+        <v>120</v>
       </c>
       <c r="Y13">
         <v>5</v>
@@ -2446,38 +2533,28 @@
       <c r="AP13">
         <v>5</v>
       </c>
-      <c r="AW13" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW13" t="s">
+        <v>60</v>
       </c>
       <c r="AX13">
         <v>1</v>
       </c>
-      <c r="AY13" t="inlineStr">
-        <is>
-          <t>rosso</t>
-        </is>
+      <c r="AY13" t="s">
+        <v>121</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:36:17</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:42:59</t>
-        </is>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>5.91.244.238</t>
-        </is>
+      <c r="D14" t="s">
+        <v>124</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -2489,12 +2566,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="2">
-        <v>45623.4881933912</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>R_2f9aMikPuRfK7O7</t>
-        </is>
+        <v>45623.488193391197</v>
+      </c>
+      <c r="I14" t="s">
+        <v>125</v>
       </c>
       <c r="N14">
         <v>37.4925</v>
@@ -2502,25 +2577,17 @@
       <c r="O14">
         <v>15.0701</v>
       </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P14" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>56</v>
+      </c>
+      <c r="R14" t="s">
+        <v>57</v>
+      </c>
+      <c r="S14" t="s">
+        <v>57</v>
       </c>
       <c r="T14">
         <v>2</v>
@@ -2534,10 +2601,8 @@
       <c r="W14">
         <v>1</v>
       </c>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>Ho imparato che bisogna mettere più contributo comune per permettere di ottenere più pascolo per le mucche</t>
-        </is>
+      <c r="X14" t="s">
+        <v>126</v>
       </c>
       <c r="Y14">
         <v>3</v>
@@ -2548,10 +2613,8 @@
       <c r="AA14">
         <v>2</v>
       </c>
-      <c r="AB14" t="inlineStr">
-        <is>
-          <t>sostenere qualcosa come una persona o un lavoro</t>
-        </is>
+      <c r="AB14" t="s">
+        <v>127</v>
       </c>
       <c r="AC14">
         <v>4</v>
@@ -2613,38 +2676,28 @@
       <c r="AV14">
         <v>6</v>
       </c>
-      <c r="AW14" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW14" t="s">
+        <v>60</v>
       </c>
       <c r="AX14">
         <v>1</v>
       </c>
-      <c r="AY14" t="inlineStr">
-        <is>
-          <t>blu</t>
-        </is>
+      <c r="AY14" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:36:27</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:43:02</t>
-        </is>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>128</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>151.43.218.225</t>
-        </is>
+      <c r="D15" t="s">
+        <v>102</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -2656,12 +2709,10 @@
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>45623.48823324074</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>R_8911eoEvaZXKOBP</t>
-        </is>
+        <v>45623.488233240743</v>
+      </c>
+      <c r="I15" t="s">
+        <v>129</v>
       </c>
       <c r="N15">
         <v>43.1479</v>
@@ -2669,25 +2720,17 @@
       <c r="O15">
         <v>12.1097</v>
       </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P15" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>56</v>
+      </c>
+      <c r="R15" t="s">
+        <v>57</v>
+      </c>
+      <c r="S15" t="s">
+        <v>57</v>
       </c>
       <c r="T15">
         <v>2</v>
@@ -2770,38 +2813,28 @@
       <c r="AV15">
         <v>2</v>
       </c>
-      <c r="AW15" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW15" t="s">
+        <v>60</v>
       </c>
       <c r="AX15">
         <v>1</v>
       </c>
-      <c r="AY15" t="inlineStr">
-        <is>
-          <t>blu</t>
-        </is>
+      <c r="AY15" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:35:42</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:43:07</t>
-        </is>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>37.163.54.206</t>
-        </is>
+      <c r="D16" t="s">
+        <v>131</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -2813,12 +2846,10 @@
         <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>45623.48828178241</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>R_27GVr9grygv7n21</t>
-        </is>
+        <v>45623.488281782411</v>
+      </c>
+      <c r="I16" t="s">
+        <v>132</v>
       </c>
       <c r="N16">
         <v>43.1479</v>
@@ -2826,25 +2857,17 @@
       <c r="O16">
         <v>12.1097</v>
       </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P16" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>56</v>
+      </c>
+      <c r="R16" t="s">
+        <v>57</v>
+      </c>
+      <c r="S16" t="s">
+        <v>57</v>
       </c>
       <c r="T16">
         <v>2</v>
@@ -2858,11 +2881,8 @@
       <c r="W16">
         <v>1</v>
       </c>
-      <c r="X16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ho imparato che bisogna mettere più contributo comune per permettere di ottenere più pascolo. _x000D_
-</t>
-        </is>
+      <c r="X16" t="s">
+        <v>133</v>
       </c>
       <c r="Y16">
         <v>3</v>
@@ -2873,10 +2893,8 @@
       <c r="AA16">
         <v>2</v>
       </c>
-      <c r="AB16" t="inlineStr">
-        <is>
-          <t>Sostenere, una persona, un lavoro o un progetto</t>
-        </is>
+      <c r="AB16" t="s">
+        <v>134</v>
       </c>
       <c r="AC16">
         <v>3</v>
@@ -2938,38 +2956,28 @@
       <c r="AV16">
         <v>6</v>
       </c>
-      <c r="AW16" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW16" t="s">
+        <v>60</v>
       </c>
       <c r="AX16">
         <v>1</v>
       </c>
-      <c r="AY16" t="inlineStr">
-        <is>
-          <t>blu</t>
-        </is>
+      <c r="AY16" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:40:08</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2024-11-27 11:43:13</t>
-        </is>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>78.211.195.11</t>
-        </is>
+      <c r="D17" t="s">
+        <v>137</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -2981,12 +2989,10 @@
         <v>1</v>
       </c>
       <c r="H17" s="2">
-        <v>45623.48835773148</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>R_8d9Mo3ypBC1zTUJ</t>
-        </is>
+        <v>45623.488357731483</v>
+      </c>
+      <c r="I17" t="s">
+        <v>138</v>
       </c>
       <c r="N17">
         <v>43.1479</v>
@@ -2994,25 +3000,17 @@
       <c r="O17">
         <v>12.1097</v>
       </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>anonymous</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="P17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>56</v>
+      </c>
+      <c r="R17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S17" t="s">
+        <v>57</v>
       </c>
       <c r="T17">
         <v>5</v>
@@ -3026,10 +3024,8 @@
       <c r="W17">
         <v>1</v>
       </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>Che si deve collaborare di più con i compagni</t>
-        </is>
+      <c r="X17" t="s">
+        <v>139</v>
       </c>
       <c r="Y17">
         <v>2</v>
@@ -3058,18 +3054,148 @@
       <c r="AP17">
         <v>3</v>
       </c>
-      <c r="AW17" t="inlineStr">
-        <is>
-          <t>BR03</t>
-        </is>
+      <c r="AW17" t="s">
+        <v>60</v>
       </c>
       <c r="AX17">
         <v>1</v>
       </c>
-      <c r="AY17" t="inlineStr">
-        <is>
-          <t>rosso</t>
-        </is>
+      <c r="AY17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>45623.488357731483</v>
+      </c>
+      <c r="I18" t="s">
+        <v>140</v>
+      </c>
+      <c r="P18" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>56</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>5</v>
+      </c>
+      <c r="U18">
+        <v>3</v>
+      </c>
+      <c r="V18">
+        <v>4</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y18">
+        <v>5</v>
+      </c>
+      <c r="Z18">
+        <v>3</v>
+      </c>
+      <c r="AA18">
+        <v>5</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC18">
+        <v>5</v>
+      </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AE18">
+        <v>2</v>
+      </c>
+      <c r="AF18">
+        <v>3</v>
+      </c>
+      <c r="AG18">
+        <v>4</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AI18">
+        <v>2</v>
+      </c>
+      <c r="AJ18">
+        <v>1</v>
+      </c>
+      <c r="AL18">
+        <v>5</v>
+      </c>
+      <c r="AM18">
+        <v>5</v>
+      </c>
+      <c r="AN18">
+        <v>4</v>
+      </c>
+      <c r="AO18">
+        <v>3</v>
+      </c>
+      <c r="AP18">
+        <v>2</v>
+      </c>
+      <c r="AQ18">
+        <v>5</v>
+      </c>
+      <c r="AR18">
+        <v>2</v>
+      </c>
+      <c r="AS18">
+        <v>4</v>
+      </c>
+      <c r="AT18">
+        <v>3</v>
+      </c>
+      <c r="AU18">
+        <v>3</v>
+      </c>
+      <c r="AV18">
+        <v>2</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX18">
+        <v>0</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>